<commit_message>
updating analysis and plots
</commit_message>
<xml_diff>
--- a/data/stations/station-master.xlsx
+++ b/data/stations/station-master.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2833" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="1129">
   <si>
     <t>19th &amp; New Hampshire Ave NW Dupont Circle south</t>
   </si>
@@ -3289,6 +3289,9 @@
     <t>Station Number in Our Data?</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
@@ -3413,6 +3416,10 @@
   </si>
   <si>
     <t>same station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allbikex$start_station[allbikex$start_station == "11th &amp; K St NW"] &lt;- "10th &amp; K St NW"
+</t>
   </si>
 </sst>
 </file>
@@ -6357,7 +6364,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B1" t="s">
         <v>62</v>
@@ -23489,15 +23496,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="44.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1078</v>
       </c>
@@ -23511,7 +23521,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -23519,13 +23529,24 @@
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="D2" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1087</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE("allbike$start_station[allbike$start_station == """,A2,"""] &lt;- """,B2,"""")</f>
+        <v>allbike$start_station[allbike$start_station == "11th &amp; K St NW"] &lt;- "10th &amp; K St NW"</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE("allbike$end_station[allbike$end_station == """,A2,"""] &lt;- """,B2,"""")</f>
+        <v>allbike$end_station[allbike$end_station == "11th &amp; K St NW"] &lt;- "10th &amp; K St NW"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -23536,10 +23557,18 @@
         <v>31001</v>
       </c>
       <c r="D3" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1089</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F63" si="0">CONCATENATE("allbike$start_station[allbike$start_station == """,A3,"""] &lt;- """,B3,"""")</f>
+        <v>allbike$start_station[allbike$start_station == "12th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G63" si="1">CONCATENATE("allbike$end_station[allbike$end_station == """,A3,"""] &lt;- """,B3,"""")</f>
+        <v>allbike$end_station[allbike$end_station == "12th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -23547,10 +23576,18 @@
         <v>450</v>
       </c>
       <c r="D4" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1088</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "12th &amp; Hayes St /  Pentagon City Metro"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "12th &amp; Hayes St /  Pentagon City Metro"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -23558,13 +23595,21 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="D5" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1090</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "13th &amp; U St NW"] &lt;- "12th &amp; U St NW"</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "13th &amp; U St NW"] &lt;- "12th &amp; U St NW"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -23575,10 +23620,18 @@
         <v>31005</v>
       </c>
       <c r="D6" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1091</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "15th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "15th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -23589,10 +23642,18 @@
         <v>31229</v>
       </c>
       <c r="D7" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1092</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "16th &amp; U St NW"] &lt;- "New Hampshire Ave &amp; T St NW"</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "16th &amp; U St NW"] &lt;- "New Hampshire Ave &amp; T St NW"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -23603,10 +23664,18 @@
         <v>31213</v>
       </c>
       <c r="D8" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1092</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "17th &amp; K St NW [formerly 17th &amp; L St NW]"] &lt;- "17th &amp; K St NW"</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "17th &amp; K St NW [formerly 17th &amp; L St NW]"] &lt;- "17th &amp; K St NW"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -23617,10 +23686,18 @@
         <v>31239</v>
       </c>
       <c r="D9" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1093</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "17th &amp; Rhode Island Ave NW"] &lt;- "Rhode Island &amp; Connecticut Ave NW"</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "17th &amp; Rhode Island Ave NW"] &lt;- "Rhode Island &amp; Connecticut Ave NW"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -23631,10 +23708,18 @@
         <v>31007</v>
       </c>
       <c r="D10" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1094</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "18th &amp; Bell St"] &lt;- "Crystal City Metro / 18th &amp; Bell St"</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "18th &amp; Bell St"] &lt;- "Crystal City Metro / 18th &amp; Bell St"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -23645,10 +23730,18 @@
         <v>31004</v>
       </c>
       <c r="D11" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1094</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "18th &amp; Hayes St"] &lt;- "Aurora Hills Community Ctr/18th &amp; Hayes St"</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "18th &amp; Hayes St"] &lt;- "Aurora Hills Community Ctr/18th &amp; Hayes St"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -23659,10 +23752,18 @@
         <v>31114</v>
       </c>
       <c r="D12" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1095</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "18th &amp; Wyoming Ave NW"] &lt;- "18th St &amp; Wyoming Ave NW"</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "18th &amp; Wyoming Ave NW"] &lt;- "18th St &amp; Wyoming Ave NW"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -23673,10 +23774,18 @@
         <v>31234</v>
       </c>
       <c r="D13" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1096</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "19th &amp; New Hampshire Ave NW Dupont Circle south"] &lt;- "20th &amp; O St NW / Dupont South"</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "19th &amp; New Hampshire Ave NW Dupont Circle south"] &lt;- "20th &amp; O St NW / Dupont South"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -23687,10 +23796,18 @@
         <v>31209</v>
       </c>
       <c r="D14" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1095</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "1st &amp; N ST SE"] &lt;- "1st &amp; N St  SE"</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "1st &amp; N ST SE"] &lt;- "1st &amp; N St  SE"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -23698,10 +23815,18 @@
         <v>313</v>
       </c>
       <c r="D15" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1097</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "20th &amp; Bell St"] &lt;- "Crystal City Metro / 18th &amp; Bell St"</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "20th &amp; Bell St"] &lt;- "Crystal City Metro / 18th &amp; Bell St"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -23709,10 +23834,18 @@
         <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1098</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "22nd &amp; Eads St"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "22nd &amp; Eads St"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -23723,10 +23856,18 @@
         <v>31013</v>
       </c>
       <c r="D17" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1099</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "23rd &amp; Eads"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "23rd &amp; Eads"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -23737,10 +23878,18 @@
         <v>31013</v>
       </c>
       <c r="D18" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1099</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "23rd &amp; Eads St"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "23rd &amp; Eads St"] &lt;- "Eads &amp; 22nd St S"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -23751,10 +23900,18 @@
         <v>31012</v>
       </c>
       <c r="D19" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "26th &amp; Crystal Dr"] &lt;- "26th &amp; S Clark St"</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "26th &amp; Crystal Dr"] &lt;- "26th &amp; S Clark St"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -23765,10 +23922,18 @@
         <v>31314</v>
       </c>
       <c r="D20" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1101</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "33rd &amp; Water St NW"] &lt;- "34th &amp; Water St NW"</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "33rd &amp; Water St NW"] &lt;- "34th &amp; Water St NW"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -23776,10 +23941,18 @@
         <v>465</v>
       </c>
       <c r="D21" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1102</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "34th St &amp; Minnesota Ave SE"] &lt;- "Randle Circle &amp; Minnesota Ave SE"</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "34th St &amp; Minnesota Ave SE"] &lt;- "Randle Circle &amp; Minnesota Ave SE"</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -23790,10 +23963,18 @@
         <v>31500</v>
       </c>
       <c r="D22" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1103</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "4th &amp; Adams St NE"] &lt;- "4th &amp; W St NE"</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "4th &amp; Adams St NE"] &lt;- "4th &amp; W St NE"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -23804,10 +23985,18 @@
         <v>31403</v>
       </c>
       <c r="D23" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1103</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "4th &amp; Kennedy St NW"] &lt;- "5th &amp; Kennedy St NW"</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "4th &amp; Kennedy St NW"] &lt;- "5th &amp; Kennedy St NW"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -23818,10 +24007,18 @@
         <v>31604</v>
       </c>
       <c r="D24" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1101</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "4th St &amp; Massachusetts Ave NW"] &lt;- "3rd &amp; H St NW"</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "4th St &amp; Massachusetts Ave NW"] &lt;- "3rd &amp; H St NW"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -23832,10 +24029,18 @@
         <v>31500</v>
       </c>
       <c r="D25" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1104</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "4th St &amp; Rhode Island Ave NE"] &lt;- "4th &amp; W St NE"</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "4th St &amp; Rhode Island Ave NE"] &lt;- "4th &amp; W St NE"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -23843,10 +24048,18 @@
         <v>236</v>
       </c>
       <c r="D26" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1105</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "5th St &amp; K St NW"] &lt;- "5th &amp; K St NW"</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "5th St &amp; K St NW"] &lt;- "5th &amp; K St NW"</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -23854,10 +24067,18 @@
         <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1106</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "6th &amp; Water St SW / SW Waterfront"] &lt;- "Maine Ave &amp; 7th St SW"</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "6th &amp; Water St SW / SW Waterfront"] &lt;- "Maine Ave &amp; 7th St SW"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -23865,10 +24086,18 @@
         <v>245</v>
       </c>
       <c r="D28" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1106</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "7th &amp; F St NW / National Portrait Gallery"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "7th &amp; F St NW / National Portrait Gallery"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -23876,10 +24105,18 @@
         <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1106</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "7th &amp; Water St SW / SW Waterfront"] &lt;- "Maine Ave &amp; 7th St SW"</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "7th &amp; Water St SW / SW Waterfront"] &lt;- "Maine Ave &amp; 7th St SW"</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -23887,10 +24124,18 @@
         <v>245</v>
       </c>
       <c r="D30" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1103</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "8th &amp; F St NW"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "8th &amp; F St NW"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -23898,26 +24143,46 @@
         <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1105</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "8th &amp; F St NW / National Portrait Gallery"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "8th &amp; F St NW / National Portrait Gallery"] &lt;- "7th &amp; F St NW/Portrait Gallery"</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1108</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1108</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -23925,21 +24190,35 @@
         <v>274</v>
       </c>
       <c r="D34" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1109</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Bethesda Ave &amp; Arlington Blvd"] &lt;- "Bethesda Ave &amp; Arlington Rd"</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Bethesda Ave &amp; Arlington Blvd"] &lt;- "Bethesda Ave &amp; Arlington Rd"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="E35" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1111</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -23947,10 +24226,18 @@
         <v>287</v>
       </c>
       <c r="D36" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1112</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Central Library"] &lt;- "Central Library / N Quincy St &amp; 10th St N"</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Central Library"] &lt;- "Central Library / N Quincy St &amp; 10th St N"</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -23958,10 +24245,18 @@
         <v>302</v>
       </c>
       <c r="D37" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1112</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Connecticut Ave &amp; Nebraska Ave NW"] &lt;- "Connecticut &amp; Nebraska Ave NW"</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Connecticut Ave &amp; Nebraska Ave NW"] &lt;- "Connecticut &amp; Nebraska Ave NW"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -23969,10 +24264,18 @@
         <v>541</v>
       </c>
       <c r="D38" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1113</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Court House Metro / Wilson Blvd &amp; N Uhle St"] &lt;- "Wilson Blvd &amp; N Uhle St"</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Court House Metro / Wilson Blvd &amp; N Uhle St"] &lt;- "Wilson Blvd &amp; N Uhle St"</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -23980,10 +24283,18 @@
         <v>352</v>
       </c>
       <c r="D39" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1114</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Fairfax Dr &amp; Glebe Rd"] &lt;- "Glebe Rd &amp; 11th St N"</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Fairfax Dr &amp; Glebe Rd"] &lt;- "Glebe Rd &amp; 11th St N"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -23991,10 +24302,18 @@
         <v>331</v>
       </c>
       <c r="D40" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1115</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Fallsgove Dr &amp; W Montgomery Ave"] &lt;- "Fallsgrove Dr &amp; W Montgomery Ave"</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Fallsgove Dr &amp; W Montgomery Ave"] &lt;- "Fallsgrove Dr &amp; W Montgomery Ave"</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -24005,10 +24324,18 @@
         <v>32022</v>
       </c>
       <c r="D41" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1116</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Garland Ave &amp; Walden Rd"] &lt;- "Dennis &amp; Amherst Ave"</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Garland Ave &amp; Walden Rd"] &lt;- "Dennis &amp; Amherst Ave"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -24016,10 +24343,18 @@
         <v>545</v>
       </c>
       <c r="D42" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1117</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Idaho Ave &amp; Newark St NW [on 2nd District patio]"] &lt;- "Wisconsin Ave &amp; Newark St NW"</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Idaho Ave &amp; Newark St NW [on 2nd District patio]"] &lt;- "Wisconsin Ave &amp; Newark St NW"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -24027,10 +24362,18 @@
         <v>376</v>
       </c>
       <c r="D43" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1118</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "King St Metro"] &lt;- "King St Metro North / Cameron St"</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "King St Metro"] &lt;- "King St Metro North / Cameron St"</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -24038,10 +24381,18 @@
         <v>384</v>
       </c>
       <c r="D44" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1119</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Lee Hwy &amp; N Nelson St"] &lt;- "Lee Hwy &amp; N Monroe St"</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Lee Hwy &amp; N Nelson St"] &lt;- "Lee Hwy &amp; N Monroe St"</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -24049,10 +24400,18 @@
         <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1120</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "McPherson Square - 14th &amp; H St NW"] &lt;- "14th St &amp; New York Ave NW"</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "McPherson Square - 14th &amp; H St NW"] &lt;- "14th St &amp; New York Ave NW"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -24060,10 +24419,18 @@
         <v>139</v>
       </c>
       <c r="D46" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1120</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "McPherson Square / 14th &amp; H St NW"] &lt;- "14th St &amp; New York Ave NW"</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "McPherson Square / 14th &amp; H St NW"] &lt;- "14th St &amp; New York Ave NW"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -24071,10 +24438,18 @@
         <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1120</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "MLK Library/9th &amp; G St NW"] &lt;- "10th &amp; G St NW"</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "MLK Library/9th &amp; G St NW"] &lt;- "10th &amp; G St NW"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -24082,10 +24457,18 @@
         <v>381</v>
       </c>
       <c r="D48" t="s">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1121</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "N Adams St &amp; Lee Hwy"] &lt;- "Lee Hwy &amp; N Adams St"</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "N Adams St &amp; Lee Hwy"] &lt;- "Lee Hwy &amp; N Adams St"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -24093,10 +24476,18 @@
         <v>288</v>
       </c>
       <c r="D49" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1122</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "N Fillmore St &amp; Clarendon Blvd"] &lt;- "Clarendon Blvd &amp; N Fillmore St"</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "N Fillmore St &amp; Clarendon Blvd"] &lt;- "Clarendon Blvd &amp; N Fillmore St"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -24104,10 +24495,18 @@
         <v>290</v>
       </c>
       <c r="D50" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1123</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "N Highland St &amp; Wilson Blvd"] &lt;- "Clarendon Metro / Wilson Blvd &amp; N Highland St"</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "N Highland St &amp; Wilson Blvd"] &lt;- "Clarendon Metro / Wilson Blvd &amp; N Highland St"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -24115,10 +24514,18 @@
         <v>384</v>
       </c>
       <c r="D51" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1124</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "N Nelson St &amp; Lee Hwy"] &lt;- "Lee Hwy &amp; N Monroe St"</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "N Nelson St &amp; Lee Hwy"] &lt;- "Lee Hwy &amp; N Monroe St"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -24126,18 +24533,32 @@
         <v>540</v>
       </c>
       <c r="D52" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1123</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "N Quincy St &amp; Wilson Blvd"] &lt;- "Wilson Blvd &amp; N Quincy St"</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "N Quincy St &amp; Wilson Blvd"] &lt;- "Wilson Blvd &amp; N Quincy St"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1125</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -24145,10 +24566,18 @@
         <v>432</v>
       </c>
       <c r="D54" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1123</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "New Hampshire Ave &amp; T St NW [formerly 16th &amp; U St NW]"] &lt;- "New Hampshire Ave &amp; T St NW"</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "New Hampshire Ave &amp; T St NW [formerly 16th &amp; U St NW]"] &lt;- "New Hampshire Ave &amp; T St NW"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -24156,10 +24585,18 @@
         <v>450</v>
       </c>
       <c r="D55" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1123</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Pentagon City Metro / 12th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Pentagon City Metro / 12th &amp; Hayes St"] &lt;- "Pentagon City Metro / 12th &amp; S Hayes St"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -24167,10 +24604,18 @@
         <v>465</v>
       </c>
       <c r="D56" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1126</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Randle Circle &amp; Minnesota Ave NE"] &lt;- "Randle Circle &amp; Minnesota Ave SE"</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Randle Circle &amp; Minnesota Ave NE"] &lt;- "Randle Circle &amp; Minnesota Ave SE"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -24178,10 +24623,18 @@
         <v>489</v>
       </c>
       <c r="D57" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1104</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "S Abingdon St &amp; 36th St S"] &lt;- "S Stafford &amp; 34th St S"</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "S Abingdon St &amp; 36th St S"] &lt;- "S Stafford &amp; 34th St S"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -24189,10 +24642,18 @@
         <v>499</v>
       </c>
       <c r="D58" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1127</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Smithsonian / Jefferson Dr &amp; 12th St SW"] &lt;- "Smithsonian-National Mall / Jefferson Dr &amp; 12th St SW"</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Smithsonian / Jefferson Dr &amp; 12th St SW"] &lt;- "Smithsonian-National Mall / Jefferson Dr &amp; 12th St SW"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -24200,10 +24661,18 @@
         <v>357</v>
       </c>
       <c r="D59" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1104</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Solutions &amp; Greensboro Dr"] &lt;- "Greensboro &amp; International Dr"</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Solutions &amp; Greensboro Dr"] &lt;- "Greensboro &amp; International Dr"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -24211,10 +24680,18 @@
         <v>511</v>
       </c>
       <c r="D60" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1119</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Thomas Jefferson Cmty Ctr / 2nd St S &amp; Ivy"] &lt;- "TJ Cmty Ctr / 2nd St &amp; S Old Glebe Rd"</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Thomas Jefferson Cmty Ctr / 2nd St S &amp; Ivy"] &lt;- "TJ Cmty Ctr / 2nd St &amp; S Old Glebe Rd"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -24222,10 +24699,18 @@
         <v>524</v>
       </c>
       <c r="D61" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1126</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Virginia Square"] &lt;- "Virginia Square Metro / N Monroe St &amp; 9th St N"</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Virginia Square"] &lt;- "Virginia Square Metro / N Monroe St &amp; 9th St N"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -24233,10 +24718,18 @@
         <v>524</v>
       </c>
       <c r="D62" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1126</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Wilson Blvd &amp; N Oakland St"] &lt;- "Virginia Square Metro / N Monroe St &amp; 9th St N"</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Wilson Blvd &amp; N Oakland St"] &lt;- "Virginia Square Metro / N Monroe St &amp; 9th St N"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>38</v>
       </c>
@@ -24244,7 +24737,15 @@
         <v>545</v>
       </c>
       <c r="D63" t="s">
-        <v>1103</v>
+        <v>1104</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>allbike$start_station[allbike$start_station == "Wisconsin Ave &amp; Macomb St NW"] &lt;- "Wisconsin Ave &amp; Newark St NW"</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>allbike$end_station[allbike$end_station == "Wisconsin Ave &amp; Macomb St NW"] &lt;- "Wisconsin Ave &amp; Newark St NW"</v>
       </c>
     </row>
   </sheetData>

</xml_diff>